<commit_message>
KC Update visualize groups method
</commit_message>
<xml_diff>
--- a/plan_dla_studentow.xlsx
+++ b/plan_dla_studentow.xlsx
@@ -495,19 +495,14 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+          <t>Analiza_matematyczna_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
         </is>
       </c>
     </row>
@@ -517,7 +512,12 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
         <is>
           <t>Technologie_informatyczne_I_laboratories_1_grp_1</t>
         </is>
@@ -531,7 +531,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -541,9 +551,9 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -553,14 +563,14 @@
           <t>16-18</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
+          <t>Analiza_matematyczna_I_lecture_2</t>
         </is>
       </c>
     </row>
@@ -568,16 +578,6 @@
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>18-20</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
         </is>
       </c>
     </row>
@@ -633,14 +633,14 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
         </is>
       </c>
     </row>
@@ -657,14 +657,14 @@
           <t>12-14</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
         </is>
       </c>
     </row>
@@ -674,9 +674,9 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -686,24 +686,19 @@
           <t>16-18</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
+          <t>Analiza_matematyczna_I_lecture_2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
+          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -713,9 +708,14 @@
           <t>18-20</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
+        </is>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
dodany genetic_cycle, metoda execute, sortowanie wg. fitness, testy zdane
</commit_message>
<xml_diff>
--- a/plan_dla_studentow.xlsx
+++ b/plan_dla_studentow.xlsx
@@ -11,6 +11,12 @@
     <sheet name="matematyka stosowana_1_2" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="matematyka stosowana_2_1" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="matematyka stosowana_2_2" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="matematyka stosowana_3_1" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="matematyka stosowana_3_2" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="matematyka stosowana_4_1" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="matematyka stosowana_4_2" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="matematyka stosowana_5_1" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="matematyka stosowana_6_1" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -448,6 +454,301 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Etyka_zawodowa_i_ochrona_własności_intelektualnej_lecture_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Podstawy_zarządzania_projektami_laboratories_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wstęp_do_analizy_funkcjonalnej_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Moduł_sumatywny_laboratories_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Systemy_baz_danych_laboratories_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Podstawy_analizy_cyklu_życia_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Wstęp_do_analizy_funkcjonalnej_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Systemy_baz_danych_lecture_1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Moduł_sumatywny_laboratories_2_grp_1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_algebry_i_geometrii_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_statystyki_matematycznej_lecture_1</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_teorii_miary_i_całki_lecture_1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Seminarium_dyplomowe_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_teorii_miary_i_całki_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_analizy_matematycznej_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Seminarium_dyplomowe_practicals_2_grp_1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_analizy_matematycznej_lecture_1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Historia_i_filozofia_odkryć_matematycznych_lecture_1</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_statystyki_matematycznej_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_algebry_i_geometrii_practicals_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -495,7 +796,7 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_1</t>
         </is>
@@ -507,14 +808,14 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+          <t>Technologie_informatyczne_I_laboratories_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -526,12 +827,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Technologie_informatyczne_I_laboratories_1_grp_1</t>
+          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+          <t>Analiza_matematyczna_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -541,11 +847,6 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -555,17 +856,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
+          <t>Analiza_matematyczna_I_lecture_2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
         </is>
       </c>
     </row>
@@ -575,9 +871,14 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -633,9 +934,9 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -645,14 +946,14 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -664,7 +965,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+          <t>Analiza_matematyczna_I_lecture_1</t>
         </is>
       </c>
     </row>
@@ -674,14 +975,9 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
-        </is>
-      </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
+          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
         </is>
       </c>
     </row>
@@ -693,12 +989,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
+          <t>Analiza_matematyczna_I_lecture_2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
         </is>
       </c>
     </row>
@@ -708,14 +1004,19 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -771,14 +1072,14 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_1</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_2_grp_1</t>
         </is>
       </c>
     </row>
@@ -788,14 +1089,14 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Podstawy_probabilistyki_practicals_1_grp_1</t>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -805,6 +1106,16 @@
           <t>12-14</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_lecture_1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_lecture_1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -814,12 +1125,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_practicals_2_grp_1</t>
+          <t>Podstawy_probabilistyki_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -829,12 +1140,7 @@
           <t>16-18</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Technologie_informatyczne_II_laboratories_1_grp_1</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Podstawy_ekonomii_i_przedsiębiorczości_lecture_1</t>
         </is>
@@ -846,24 +1152,19 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_1</t>
-        </is>
-      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Podstawy_probabilistyki_lecture_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_1</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
           <t>Analiza_matematyczna_II_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_II_laboratories_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -921,23 +1222,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_II_practicals_2_grp_2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -947,19 +1242,16 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Podstawy_probabilistyki_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_II_laboratories_1_grp_2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -967,15 +1259,16 @@
           <t>12-14</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_lecture_1</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Technologie_informatyczne_II_laboratories_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
+          <t>Analiza_matematyczna_II_lecture_1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -983,19 +1276,16 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_practicals_1_grp_2</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr"/>
+          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_2</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1003,19 +1293,16 @@
           <t>16-18</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr">
+      <c r="B6" t="inlineStr">
         <is>
           <t>Podstawy_ekonomii_i_przedsiębiorczości_lecture_1</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_2_grp_2</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1023,15 +1310,663 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Wstęp_do_teorii_miary_i_całki_lecture_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_lecture_2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Wstęp_do_matematyki_finansowej_i_ubezpieczeniowej_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Algebra_abstrakcyjna_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Wstęp_do_teorii_miary_i_całki_practicals_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Algebra_abstrakcyjna_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_matematyki_finansowej_i_ubezpieczeniowej_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_practicals_2_grp_1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Wstęp_do_teorii_miary_i_całki_lecture_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_lecture_2</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Wstęp_do_matematyki_finansowej_i_ubezpieczeniowej_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_lecture_1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_practicals_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_laboratories_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Algebra_abstrakcyjna_lecture_1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Algebra_abstrakcyjna_practicals_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Wstęp_do_matematyki_finansowej_i_ubezpieczeniowej_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Podstawy_statystyki_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_III_practicals_2_grp_2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_teorii_miary_i_całki_practicals_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Programowanie_obiektowe_w_języku_Java_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_miary_i_kategorii_lecture_2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Funkcje_zespolone_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Programowanie_obiektowe_w_języku_Java_lecture_1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Finanse_osobiste_laboratories_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Wprowadzenie_do_szeregów_czasowych_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_miary_i_kategorii_lecture_1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Wprowadzenie_do_szeregów_czasowych_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Funkcje_zespolone_lecture_1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Teoria_liczb_z_zastosowaniami_w_kryptografii_lecture_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Podstawy_programowania_w_VBA_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Wstęp_do_równań_różniczkowych_practicals_1_grp_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Elementy_kombinatoryki_i_teorii_grafów_lecture_1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Teoria_liczb_z_zastosowaniami_w_kryptografii_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Elementy_kombinatoryki_i_teorii_grafów_practicals_1_grp_1</t>
+        </is>
+      </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Podstawy_probabilistyki_lecture_1</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+          <t>Podstawy_programowania_w_VBA_lecture_1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_równań_różniczkowych_lecture_1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Poniedziałek</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Wtorek</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Środa</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Czwartek</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Piątek</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>8-10</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_miary_i_kategorii_lecture_2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Funkcje_zespolone_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Programowanie_obiektowe_w_języku_Java_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>10-12</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Wstęp_do_równań_różniczkowych_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Wybrane_zagadnienia_miary_i_kategorii_lecture_1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Wprowadzenie_do_szeregów_czasowych_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>12-14</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Funkcje_zespolone_lecture_1</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Teoria_liczb_z_zastosowaniami_w_kryptografii_lecture_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>14-16</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Finanse_osobiste_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Elementy_kombinatoryki_i_teorii_grafów_practicals_1_grp_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>16-18</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Podstawy_programowania_w_VBA_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Elementy_kombinatoryki_i_teorii_grafów_lecture_1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Teoria_liczb_z_zastosowaniami_w_kryptografii_lecture_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>18-20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Programowanie_obiektowe_w_języku_Java_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Podstawy_programowania_w_VBA_lecture_1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_równań_różniczkowych_lecture_1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Wprowadzenie_do_szeregów_czasowych_practicals_1_grp_2</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
KC Quick fixes (#14)
</commit_message>
<xml_diff>
--- a/plan_dla_studentow.xlsx
+++ b/plan_dla_studentow.xlsx
@@ -495,11 +495,6 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -507,19 +502,9 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_lecture_1</t>
         </is>
       </c>
     </row>
@@ -529,6 +514,16 @@
           <t>12-14</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_2_grp_1</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -536,19 +531,19 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_1</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
         </is>
       </c>
     </row>
@@ -558,11 +553,6 @@
           <t>16-18</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -570,14 +560,24 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_lecture_2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>Technologie_informatyczne_I_laboratories_1_grp_1</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -633,9 +633,9 @@
           <t>8-10</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -647,12 +647,12 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
+          <t>Analiza_matematyczna_I_lecture_1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
         </is>
       </c>
     </row>
@@ -662,11 +662,6 @@
           <t>12-14</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -674,19 +669,14 @@
           <t>14-16</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_lecture_1</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
-        </is>
-      </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_practicals_2_grp_2</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_lecture_1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_lecture_1</t>
         </is>
       </c>
     </row>
@@ -696,19 +686,19 @@
           <t>16-18</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_practicals_1_grp_2</t>
+        </is>
+      </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_I_lecture_2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Wstęp_do_obliczeń_symbolicznych_laboratories_1_grp_2</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_I_practicals_1_grp_2</t>
+          <t>Wstęp_do_logiki_i_teorii_mnogości_practicals_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -716,6 +706,16 @@
       <c r="A7" s="1" t="inlineStr">
         <is>
           <t>18-20</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_I_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_I_lecture_2</t>
         </is>
       </c>
     </row>
@@ -771,9 +771,14 @@
           <t>8-10</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_2_grp_1</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
+          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -783,14 +788,19 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Podstawy_probabilistyki_practicals_1_grp_1</t>
-        </is>
-      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_1</t>
+          <t>Analiza_matematyczna_II_lecture_1</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_lecture_1</t>
         </is>
       </c>
     </row>
@@ -800,29 +810,9 @@
           <t>12-14</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>Podstawy_ekonomii_i_przedsiębiorczości_lecture_1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Technologie_informatyczne_II_laboratories_1_grp_1</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_1</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -832,9 +822,24 @@
           <t>14-16</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_II_laboratories_1_grp_1</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Podstawy_probabilistyki_lecture_1</t>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_1</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
         </is>
       </c>
     </row>
@@ -844,11 +849,6 @@
           <t>16-18</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_practicals_2_grp_1</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -856,14 +856,14 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
-        </is>
-      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_1</t>
+          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_practicals_1_grp_1</t>
         </is>
       </c>
     </row>
@@ -922,16 +922,12 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_2</t>
+          <t>Podstawy_probabilistyki_practicals_1_grp_2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
-        </is>
-      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -939,19 +935,27 @@
           <t>10-12</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_lecture_1</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Podstawy_probabilistyki_practicals_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
+          <t>Topologia_przestrzeni_metrycznych_practicals_1_grp_2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Technologie_informatyczne_II_laboratories_1_grp_2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Podstawy_probabilistyki_lecture_1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -959,21 +963,17 @@
           <t>12-14</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
         <is>
           <t>Podstawy_ekonomii_i_przedsiębiorczości_lecture_1</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Analiza_matematyczna_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Analiza_matematyczna_II_practicals_2_grp_2</t>
+          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_2</t>
         </is>
       </c>
     </row>
@@ -986,12 +986,20 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Podstawy_probabilistyki_lecture_1</t>
+          <t>Analiza_matematyczna_II_practicals_2_grp_2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_2</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1001,16 +1009,8 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Komputerowe_obliczenia_matematyczne_laboratories_1_grp_2</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Technologie_informatyczne_II_laboratories_1_grp_2</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -1019,19 +1019,19 @@
           <t>18-20</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_lecture_1</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Algebra_liniowa_z_geometrią_analityczną_II_practicals_1_grp_2</t>
-        </is>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Topologia_przestrzeni_metrycznych_lecture_1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Analiza_matematyczna_II_practicals_1_grp_2</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>